<commit_message>
[VM:timothy.queen@5/14/2015 10:20:48 AM] updated lessons learned
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C14095
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoachingLog Lessons Learned.xlsx
+++ b/Project Management/CCO OY2_eCoachingLog Lessons Learned.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="108" windowWidth="15168" windowHeight="9360"/>
+    <workbookView xWindow="90" yWindow="105" windowWidth="15165" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Performance Management Lessons Learned</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Title</t>
   </si>
@@ -61,6 +58,21 @@
   </si>
   <si>
     <t>Inception</t>
+  </si>
+  <si>
+    <t>Regression testing should be performed when major changes are made</t>
+  </si>
+  <si>
+    <t>Changes made to one part of the system may have a negative impact on other parts of the system</t>
+  </si>
+  <si>
+    <t>Create regression test cases that can be used when significant changes are made to eCL.</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>eCoaching Log Lessons Learned</t>
   </si>
 </sst>
 </file>
@@ -434,22 +446,22 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -459,60 +471,74 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>41820</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="3"/>
+      <c r="B4" s="2">
+        <v>42138</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -529,7 +555,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -541,25 +567,25 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -677,14 +703,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A2E50BB-E3BE-4950-9E56-B46F5DB14F70}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E0F7557-C740-455B-9B61-E559B145113E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -695,6 +713,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A2E50BB-E3BE-4950-9E56-B46F5DB14F70}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>